<commit_message>
latest state table spreadsheet
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB329A9D-04EF-43E4-9813-A960EA7E0B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04450E7-09A0-46D7-B176-BE7052C37889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="345" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -323,9 +323,6 @@
     <t>index</t>
   </si>
   <si>
-    <t>inputsFange</t>
-  </si>
-  <si>
     <t>storeValMasks</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>inputRBG</t>
+  </si>
+  <si>
+    <t>inputsRange</t>
   </si>
 </sst>
 </file>
@@ -771,8 +771,8 @@
   <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>29</v>
@@ -821,17 +821,17 @@
         <v>14</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>66</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="Q1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
starting to fill in pieces
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{101E8074-162F-4643-8AD7-B1AD28728C7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1BDB81-5E91-4D71-B34E-09DDB3FAE99F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="690" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="1035" yWindow="1035" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -351,19 +351,19 @@
     <t>m_EEPROM</t>
   </si>
   <si>
-    <t>mEFCT_SPCL|mEFCT_OPEN_BARREL</t>
-  </si>
-  <si>
-    <t>mEFCT_SPCL|mEFCT_LOCK_LOAD</t>
-  </si>
-  <si>
-    <t>mEFCT_SPCL|mEFCT_SHOOT</t>
-  </si>
-  <si>
     <t>mSPARKLE</t>
   </si>
   <si>
     <t>mBLINK</t>
+  </si>
+  <si>
+    <t>mEFCT_SPCLFUNC|mEFCT_SHOOT</t>
+  </si>
+  <si>
+    <t>mEFCT_SPCLFUNC|mEFCT_OPEN_BARREL</t>
+  </si>
+  <si>
+    <t>mEFCT_SPCLFUNC|mEFCT_LOCK_LOAD</t>
   </si>
 </sst>
 </file>
@@ -816,14 +816,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
@@ -896,7 +896,7 @@
         <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J2" t="s">
         <v>60</v>
@@ -981,10 +981,10 @@
         <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -1010,10 +1010,10 @@
         <v>60</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F16" t="s">
         <v>1</v>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
         <v>2</v>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
         <v>3</v>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -1311,7 +1311,7 @@
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>65</v>
       </c>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="D43" s="3"/>
       <c r="E43" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G43" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
rename some things, use EEPROM config
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6A0FA2-6C1C-4881-AA70-F378B10D3925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B8FB93-228F-4E84-BEEB-BBA6243EB6B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="645" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="4245" yWindow="1335" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
   <si>
     <t>trigYellow</t>
   </si>
@@ -345,9 +345,6 @@
     <t>m_EEPROM</t>
   </si>
   <si>
-    <t>mSPARKLE</t>
-  </si>
-  <si>
     <t>mBLINK</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>efctLED</t>
+  </si>
+  <si>
+    <t>mEFCT_PWRON</t>
   </si>
 </sst>
 </file>
@@ -816,7 +816,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,6 +829,7 @@
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
@@ -848,10 +849,10 @@
         <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>55</v>
@@ -888,18 +889,21 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>58</v>
       </c>
       <c r="L2" t="s">
         <v>19</v>
@@ -943,10 +947,10 @@
         <v>58</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
@@ -981,10 +985,10 @@
         <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>11</v>
@@ -1010,10 +1014,10 @@
         <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>12</v>
@@ -1081,7 +1085,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -1105,7 +1109,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -1129,7 +1133,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -1150,7 +1154,7 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -1201,7 +1205,7 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
         <v>0</v>
@@ -1222,7 +1226,7 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
         <v>1</v>
@@ -1243,7 +1247,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -1264,7 +1268,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
@@ -1285,7 +1289,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
         <v>3</v>
@@ -1513,7 +1517,7 @@
       </c>
       <c r="D43" s="3"/>
       <c r="E43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G43" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
re-organize the mSPCL_ processing
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B8FB93-228F-4E84-BEEB-BBA6243EB6B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6A486B-DD35-48D6-8A49-8891D4192009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4245" yWindow="1335" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="111">
   <si>
     <t>trigYellow</t>
   </si>
@@ -222,9 +222,6 @@
     <t>mMENU</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>mMENUCHOICE</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>mSPCL_CONTINUOUS</t>
   </si>
   <si>
-    <t>mSPCL_ONETIME | mSPCL_SHOOT</t>
-  </si>
-  <si>
     <t>mVAL_YBG</t>
   </si>
   <si>
@@ -348,15 +342,6 @@
     <t>mBLINK</t>
   </si>
   <si>
-    <t>mEFCT_SPCLFUNC|mEFCT_SHOOT</t>
-  </si>
-  <si>
-    <t>mEFCT_SPCLFUNC|mEFCT_OPEN_BARREL</t>
-  </si>
-  <si>
-    <t>mEFCT_SPCLFUNC|mEFCT_LOCK_LOAD</t>
-  </si>
-  <si>
     <t>efctSound</t>
   </si>
   <si>
@@ -364,6 +349,33 @@
   </si>
   <si>
     <t>mEFCT_PWRON</t>
+  </si>
+  <si>
+    <t>mSPCL_EFCT_CONTINUOUS|mSPCL_HANDLER | mSPCL_HANDLER_SHOOT</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_WAITING</t>
+  </si>
+  <si>
+    <t>mSPCL_EFCT_CONTINUOUS</t>
+  </si>
+  <si>
+    <t>mOPNBRL</t>
+  </si>
+  <si>
+    <t>mLOKLOD</t>
+  </si>
+  <si>
+    <t>mEFCT_OPEN_BARREL</t>
+  </si>
+  <si>
+    <t>mEFCT_LOCK_LOAD</t>
+  </si>
+  <si>
+    <t>the door is ajar…</t>
+  </si>
+  <si>
+    <t>please fasten your seatbelts…</t>
   </si>
 </sst>
 </file>
@@ -477,7 +489,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -495,6 +507,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -816,11 +834,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" customWidth="1"/>
     <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
@@ -843,16 +863,16 @@
         <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>55</v>
@@ -886,20 +906,28 @@
         <v>16</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>58</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -912,17 +940,26 @@
         <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="3"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
       <c r="L3" t="s">
         <v>20</v>
       </c>
@@ -930,34 +967,38 @@
         <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="11"/>
       <c r="L4" t="s">
         <v>21</v>
       </c>
@@ -965,37 +1006,41 @@
         <v>35</v>
       </c>
       <c r="O4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q4" t="s">
         <v>46</v>
       </c>
       <c r="R4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="11"/>
       <c r="L5" t="s">
         <v>22</v>
       </c>
@@ -1003,14 +1048,15 @@
         <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1019,12 +1065,15 @@
       <c r="E6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="s">
-        <v>58</v>
-      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="11"/>
       <c r="L6" t="s">
         <v>23</v>
       </c>
@@ -1032,28 +1081,23 @@
         <v>37</v>
       </c>
       <c r="O6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>60</v>
-      </c>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
       <c r="L7" t="s">
         <v>24</v>
       </c>
@@ -1061,14 +1105,33 @@
         <v>38</v>
       </c>
       <c r="O7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="3"/>
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" t="s">
+        <v>109</v>
+      </c>
       <c r="L8" t="s">
         <v>25</v>
       </c>
@@ -1076,23 +1139,20 @@
         <v>39</v>
       </c>
       <c r="O8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>61</v>
-      </c>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
       <c r="L9" t="s">
         <v>26</v>
       </c>
@@ -1100,22 +1160,32 @@
         <v>40</v>
       </c>
       <c r="O9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>62</v>
+      <c r="A10" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -1124,23 +1194,10 @@
         <v>41</v>
       </c>
       <c r="O10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>63</v>
-      </c>
       <c r="L11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1149,19 +1206,6 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" t="s">
-        <v>58</v>
-      </c>
       <c r="L12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1170,7 +1214,6 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D13" s="3"/>
       <c r="L13" t="s">
         <v>30</v>
       </c>
@@ -1178,16 +1221,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>64</v>
-      </c>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1196,392 +1230,323 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D15" s="3"/>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="25" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" t="s">
+        <v>95</v>
+      </c>
+      <c r="I34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H16" t="s">
-        <v>97</v>
-      </c>
-      <c r="I16" t="s">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="J42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" t="s">
-        <v>97</v>
-      </c>
-      <c r="I17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" t="s">
-        <v>97</v>
-      </c>
-      <c r="I18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" t="s">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" t="s">
         <v>9</v>
       </c>
-      <c r="G19" t="s">
-        <v>87</v>
-      </c>
-      <c r="H19" t="s">
-        <v>97</v>
-      </c>
-      <c r="I19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="I46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="F47" t="s">
         <v>3</v>
       </c>
-      <c r="I20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="J24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="3:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="I47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="D49" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" t="s">
+        <v>86</v>
+      </c>
+      <c r="H49" t="s">
+        <v>94</v>
+      </c>
+      <c r="I49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
         <v>68</v>
       </c>
-      <c r="F28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="D50" s="3"/>
+      <c r="F50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="F29" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" t="s">
-        <v>88</v>
-      </c>
-      <c r="H31" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="F32" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="F33" t="s">
-        <v>3</v>
-      </c>
-      <c r="I33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" t="s">
-        <v>96</v>
-      </c>
-      <c r="I35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="F36" t="s">
-        <v>4</v>
-      </c>
-      <c r="I36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="F37" t="s">
-        <v>3</v>
-      </c>
-      <c r="I37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" t="s">
-        <v>90</v>
-      </c>
-      <c r="H39" t="s">
-        <v>96</v>
-      </c>
-      <c r="I39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
-      <c r="I40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="F41" t="s">
-        <v>3</v>
-      </c>
-      <c r="I41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" t="s">
-        <v>100</v>
-      </c>
-      <c r="G43" t="s">
-        <v>96</v>
-      </c>
-      <c r="H43" t="s">
-        <v>50</v>
-      </c>
-      <c r="J43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J49" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>66</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="F51" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1590,94 +1555,211 @@
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J53" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>87</v>
+      </c>
+      <c r="H53" t="s">
+        <v>94</v>
+      </c>
+      <c r="I53" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
       <c r="D54" s="3"/>
+      <c r="F54" t="s">
+        <v>4</v>
+      </c>
+      <c r="I54" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>69</v>
+      </c>
       <c r="D55" s="3"/>
+      <c r="F55" t="s">
+        <v>3</v>
+      </c>
+      <c r="I55" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D57" s="3"/>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" t="s">
+        <v>94</v>
+      </c>
+      <c r="I57" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
       <c r="D58" s="3"/>
+      <c r="F58" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
       <c r="D59" s="3"/>
+      <c r="F59" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="60" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>71</v>
+      </c>
       <c r="D61" s="3"/>
+      <c r="E61" t="s">
+        <v>98</v>
+      </c>
+      <c r="G61" t="s">
+        <v>94</v>
+      </c>
+      <c r="H61" t="s">
+        <v>50</v>
+      </c>
+      <c r="J61" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="62" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D63" s="3"/>
+    <row r="63" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J63" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="64" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>75</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D80" s="3"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finally made decision on where to put EFCT_special calls
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6A486B-DD35-48D6-8A49-8891D4192009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E74E420-B441-4C40-9B43-17BAEAA6E105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="1335" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="4590" yWindow="1680" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="111">
   <si>
     <t>trigYellow</t>
   </si>
@@ -351,12 +351,6 @@
     <t>mEFCT_PWRON</t>
   </si>
   <si>
-    <t>mSPCL_EFCT_CONTINUOUS|mSPCL_HANDLER | mSPCL_HANDLER_SHOOT</t>
-  </si>
-  <si>
-    <t>mEFCT_UNIQ_WAITING</t>
-  </si>
-  <si>
     <t>mSPCL_EFCT_CONTINUOUS</t>
   </si>
   <si>
@@ -376,6 +370,12 @@
   </si>
   <si>
     <t>please fasten your seatbelts…</t>
+  </si>
+  <si>
+    <t>mSPCL_HANDLER | mSPCL_HANDLER_SHOOT</t>
+  </si>
+  <si>
+    <t>mSPCL_EFCT_CONTINUOUS|mEFCT_UNIQ_WAITING</t>
   </si>
 </sst>
 </file>
@@ -834,7 +834,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,19 +976,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>3</v>
@@ -1018,19 +1018,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
@@ -1038,7 +1036,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J5" s="11"/>
       <c r="L5" t="s">
@@ -1051,19 +1049,17 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>12</v>
@@ -1071,7 +1067,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J6" s="11"/>
       <c r="L6" t="s">
@@ -1110,17 +1106,17 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -1130,7 +1126,7 @@
         <v>58</v>
       </c>
       <c r="K8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
@@ -1165,17 +1161,17 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -1185,7 +1181,7 @@
         <v>58</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -1234,7 +1230,7 @@
     </row>
     <row r="25" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
         <v>58</v>
@@ -1314,7 +1310,7 @@
     </row>
     <row r="32" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>60</v>
@@ -1433,7 +1429,7 @@
     </row>
     <row r="40" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
@@ -1468,7 +1464,7 @@
     </row>
     <row r="44" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
start disambiguating the mXXX_xxx #defines
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E74E420-B441-4C40-9B43-17BAEAA6E105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B7AE2D-1F0B-431C-928C-B81DA2EE897B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="1680" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="134">
   <si>
     <t>trigYellow</t>
   </si>
@@ -376,6 +377,75 @@
   </si>
   <si>
     <t>mSPCL_EFCT_CONTINUOUS|mEFCT_UNIQ_WAITING</t>
+  </si>
+  <si>
+    <t>mROW_POWERON</t>
+  </si>
+  <si>
+    <t>mROW_MENU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>mROW_OPNBRL</t>
+  </si>
+  <si>
+    <t>mROW_LOKLOD</t>
+  </si>
+  <si>
+    <t>mROW_MENUCHOICE</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SOUND</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SCHOICE</t>
+  </si>
+  <si>
+    <t>mROW_CFG_LIGHT</t>
+  </si>
+  <si>
+    <t>mROW_CFG_OTHER</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SWINDUP</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SWINDUP0</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SWINDUP1</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SWINDUP2</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SWINDUP3</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SOUNDSTORE</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SSHOOT</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SOPEN</t>
+  </si>
+  <si>
+    <t>mROW_CFG_SLOAD</t>
+  </si>
+  <si>
+    <t>mROW_CFG_LCHOICE</t>
+  </si>
+  <si>
+    <t>mROW_CFG_OCHOICE</t>
+  </si>
+  <si>
+    <t>mROW_MENUCFG</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -834,7 +904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:E6"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +985,7 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>101</v>
@@ -928,7 +998,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>51</v>
@@ -982,7 +1052,7 @@
         <v>109</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>110</v>
@@ -996,7 +1066,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="J4" s="11"/>
       <c r="L4" t="s">
@@ -1021,9 +1091,7 @@
     <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="3" t="s">
         <v>110</v>
       </c>
@@ -1036,7 +1104,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="J5" s="11"/>
       <c r="L5" t="s">
@@ -1052,9 +1120,7 @@
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="C6" s="11"/>
       <c r="D6" s="3" t="s">
         <v>110</v>
       </c>
@@ -1067,7 +1133,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="J6" s="11"/>
       <c r="L6" t="s">
@@ -1086,7 +1152,9 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -1110,7 +1178,7 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>105</v>
@@ -1123,7 +1191,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="K8" t="s">
         <v>107</v>
@@ -1141,7 +1209,9 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1165,7 +1235,7 @@
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>106</v>
@@ -1178,7 +1248,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>108</v>
@@ -1194,6 +1264,9 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
       <c r="L11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1202,6 +1275,9 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
       <c r="L12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1210,6 +1286,9 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
       <c r="L13" t="s">
         <v>30</v>
       </c>
@@ -1218,6 +1297,9 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
       <c r="L14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1226,14 +1308,62 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
       <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="25" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>18</v>
@@ -1245,9 +1375,14 @@
         <v>59</v>
       </c>
     </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" t="s">
@@ -1262,7 +1397,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" t="s">
@@ -1277,7 +1412,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" t="s">
@@ -1292,7 +1427,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" t="s">
@@ -1306,6 +1441,9 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -1313,7 +1451,7 @@
         <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>10</v>
@@ -1323,11 +1461,14 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" t="s">
@@ -1348,7 +1489,7 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" t="s">
@@ -1369,7 +1510,7 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" t="s">
@@ -1390,7 +1531,7 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" t="s">
@@ -1411,7 +1552,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" t="s">
@@ -1425,6 +1566,9 @@
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -1432,7 +1576,7 @@
         <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>8</v>
@@ -1442,11 +1586,14 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>113</v>
+      </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>7</v>
@@ -1460,6 +1607,9 @@
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>113</v>
+      </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -1467,7 +1617,7 @@
         <v>102</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>15</v>
@@ -1476,9 +1626,14 @@
         <v>67</v>
       </c>
     </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c r="F46" t="s">
         <v>9</v>
@@ -1489,7 +1644,7 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c r="D47" s="3"/>
       <c r="F47" t="s">
@@ -1500,11 +1655,14 @@
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>47</v>
@@ -1524,7 +1682,7 @@
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="D50" s="3"/>
       <c r="F50" t="s">
@@ -1536,7 +1694,7 @@
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="D51" s="3"/>
       <c r="F51" t="s">
@@ -1547,11 +1705,14 @@
       </c>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>48</v>
@@ -1571,7 +1732,7 @@
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="D54" s="3"/>
       <c r="F54" t="s">
@@ -1583,7 +1744,7 @@
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="D55" s="3"/>
       <c r="F55" t="s">
@@ -1594,11 +1755,14 @@
       </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>49</v>
@@ -1618,7 +1782,7 @@
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="D58" s="3"/>
       <c r="F58" t="s">
@@ -1630,7 +1794,7 @@
     </row>
     <row r="59" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3"/>
       <c r="F59" t="s">
@@ -1641,11 +1805,14 @@
       </c>
     </row>
     <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>113</v>
+      </c>
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" t="s">
@@ -1662,11 +1829,14 @@
       </c>
     </row>
     <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>113</v>
+      </c>
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>77</v>
@@ -1676,11 +1846,14 @@
       </c>
     </row>
     <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>113</v>
+      </c>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>78</v>
@@ -1690,11 +1863,14 @@
       </c>
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>113</v>
+      </c>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>79</v>
@@ -1704,11 +1880,14 @@
       </c>
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>113</v>
+      </c>
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>72</v>
@@ -1718,11 +1897,14 @@
       </c>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>113</v>
+      </c>
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>73</v>
@@ -1829,4 +2011,358 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECE4675-A946-4305-AAF8-D10CA956FB8A}">
+  <dimension ref="A1:B71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B71">
+    <sortCondition ref="A2:A71"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
continue moving flags to most logical position and refactoring code
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B7AE2D-1F0B-431C-928C-B81DA2EE897B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799E8FD3-6C4D-428B-BEBD-9CC6ED226826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="1680" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="134">
   <si>
     <t>trigYellow</t>
   </si>
@@ -352,6 +352,12 @@
     <t>mEFCT_PWRON</t>
   </si>
   <si>
+    <t>mSPCL_EFCT_CONTINUOUS|mSPCL_HANDLER | mSPCL_HANDLER_SHOOT</t>
+  </si>
+  <si>
+    <t>mEFCT_UNIQ_WAITING</t>
+  </si>
+  <si>
     <t>mSPCL_EFCT_CONTINUOUS</t>
   </si>
   <si>
@@ -371,12 +377,6 @@
   </si>
   <si>
     <t>please fasten your seatbelts…</t>
-  </si>
-  <si>
-    <t>mSPCL_HANDLER | mSPCL_HANDLER_SHOOT</t>
-  </si>
-  <si>
-    <t>mSPCL_EFCT_CONTINUOUS|mEFCT_UNIQ_WAITING</t>
   </si>
   <si>
     <t>mROW_POWERON</t>
@@ -904,7 +904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:J10"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,19 +1046,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>112</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>3</v>
@@ -1090,13 +1090,15 @@
     </row>
     <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
@@ -1119,13 +1121,15 @@
     </row>
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>12</v>
@@ -1174,17 +1178,17 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -1194,7 +1198,7 @@
         <v>112</v>
       </c>
       <c r="K8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
@@ -1231,17 +1235,17 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
         <v>115</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -1251,7 +1255,7 @@
         <v>112</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -1360,7 +1364,7 @@
     </row>
     <row r="25" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
         <v>132</v>
@@ -1448,7 +1452,7 @@
     </row>
     <row r="32" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
         <v>117</v>
@@ -1573,7 +1577,7 @@
     </row>
     <row r="40" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
         <v>119</v>
@@ -1614,7 +1618,7 @@
     </row>
     <row r="44" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
         <v>121</v>
@@ -2156,7 +2160,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
         <v>115</v>
@@ -2180,7 +2184,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
RBG_debuggable now makes complete *.cpp file for MS VS
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799E8FD3-6C4D-428B-BEBD-9CC6ED226826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECCE393-9CE0-4D9E-B8E9-F16479007235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="1680" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
@@ -904,7 +904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
a fair bit of reshuffling
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECCE393-9CE0-4D9E-B8E9-F16479007235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F19D18-3BD2-49AA-BE53-D225861347A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1680" windowWidth="32760" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="4590" yWindow="1680" windowWidth="32745" windowHeight="16875" activeTab="1" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="RULES" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="148">
   <si>
     <t>trigYellow</t>
   </si>
@@ -352,9 +353,6 @@
     <t>mEFCT_PWRON</t>
   </si>
   <si>
-    <t>mSPCL_EFCT_CONTINUOUS|mSPCL_HANDLER | mSPCL_HANDLER_SHOOT</t>
-  </si>
-  <si>
     <t>mEFCT_UNIQ_WAITING</t>
   </si>
   <si>
@@ -446,13 +444,58 @@
   </si>
   <si>
     <t>new</t>
+  </si>
+  <si>
+    <t>mROW_WINDUP</t>
+  </si>
+  <si>
+    <t>… and the WINDUP</t>
+  </si>
+  <si>
+    <t>mROW_WINDUP_SOUND</t>
+  </si>
+  <si>
+    <t>mEFCT_WIND_UP</t>
+  </si>
+  <si>
+    <t>mROW_SHOOT</t>
+  </si>
+  <si>
+    <t>POW!!!</t>
+  </si>
+  <si>
+    <t>mSPCL_HANDLER | mSPCL_HANDLER_SHOOT</t>
+  </si>
+  <si>
+    <t>mROW_SHOOT_SOUND</t>
+  </si>
+  <si>
+    <t>POW SOUND</t>
+  </si>
+  <si>
+    <t>mEFCT_SHOOT</t>
+  </si>
+  <si>
+    <t>mROW_SOLENOID</t>
+  </si>
+  <si>
+    <t>release solenoid</t>
+  </si>
+  <si>
+    <t>mSPCL_HANDLER | mSPCL_HANDLER_SOLENOID</t>
+  </si>
+  <si>
+    <t>MUST contain mROW_something or it will be ignored</t>
+  </si>
+  <si>
+    <t>if it is a list of input selections, make them all have the same name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,8 +539,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +567,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -553,13 +608,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -583,10 +639,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -902,9 +962,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +1045,7 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>101</v>
@@ -998,7 +1058,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>51</v>
@@ -1046,27 +1106,27 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
-        <v>112</v>
+      <c r="I4" t="s">
+        <v>133</v>
       </c>
       <c r="J4" s="11"/>
       <c r="L4" t="s">
@@ -1088,17 +1148,19 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="11"/>
+        <v>103</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>111</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
@@ -1106,7 +1168,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J5" s="11"/>
       <c r="L5" t="s">
@@ -1119,17 +1181,19 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="11"/>
+        <v>103</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>111</v>
+      </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>12</v>
@@ -1137,7 +1201,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J6" s="11"/>
       <c r="L6" t="s">
@@ -1157,7 +1221,7 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -1178,27 +1242,27 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
@@ -1214,7 +1278,7 @@
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -1235,27 +1299,27 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -1268,9 +1332,6 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>113</v>
-      </c>
       <c r="L11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1279,8 +1340,14 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>133</v>
+      </c>
+      <c r="J12" t="s">
+        <v>135</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>29</v>
@@ -1290,9 +1357,6 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>113</v>
-      </c>
       <c r="L13" t="s">
         <v>30</v>
       </c>
@@ -1302,7 +1366,16 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>113</v>
+        <v>135</v>
+      </c>
+      <c r="D14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J14" t="s">
+        <v>137</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>31</v>
@@ -1312,62 +1385,81 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>113</v>
-      </c>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="C16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="J16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="12"/>
       <c r="C18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="D18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>145</v>
+      </c>
       <c r="C21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>18</v>
@@ -1379,14 +1471,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" t="s">
@@ -1399,9 +1491,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" t="s">
@@ -1414,9 +1506,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" t="s">
@@ -1429,9 +1521,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" t="s">
@@ -1444,18 +1536,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>10</v>
@@ -1466,13 +1558,13 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" t="s">
@@ -1493,7 +1585,7 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" t="s">
@@ -1514,7 +1606,7 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" t="s">
@@ -1535,7 +1627,7 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" t="s">
@@ -1556,7 +1648,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" t="s">
@@ -1571,16 +1663,16 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>8</v>
@@ -1591,13 +1683,13 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>7</v>
@@ -1612,16 +1704,16 @@
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>15</v>
@@ -1632,12 +1724,12 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F46" t="s">
         <v>9</v>
@@ -1648,7 +1740,7 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D47" s="3"/>
       <c r="F47" t="s">
@@ -1660,13 +1752,13 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>47</v>
@@ -1686,7 +1778,7 @@
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D50" s="3"/>
       <c r="F50" t="s">
@@ -1698,7 +1790,7 @@
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D51" s="3"/>
       <c r="F51" t="s">
@@ -1710,13 +1802,13 @@
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>48</v>
@@ -1736,7 +1828,7 @@
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D54" s="3"/>
       <c r="F54" t="s">
@@ -1748,7 +1840,7 @@
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D55" s="3"/>
       <c r="F55" t="s">
@@ -1760,13 +1852,13 @@
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>49</v>
@@ -1786,7 +1878,7 @@
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D58" s="3"/>
       <c r="F58" t="s">
@@ -1798,7 +1890,7 @@
     </row>
     <row r="59" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D59" s="3"/>
       <c r="F59" t="s">
@@ -1810,13 +1902,13 @@
     </row>
     <row r="60" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" t="s">
@@ -1834,13 +1926,13 @@
     </row>
     <row r="62" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>77</v>
@@ -1851,13 +1943,13 @@
     </row>
     <row r="64" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>78</v>
@@ -1868,13 +1960,13 @@
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>79</v>
@@ -1885,13 +1977,13 @@
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>72</v>
@@ -1902,13 +1994,13 @@
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>73</v>
@@ -2018,6 +2110,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E088660E-D1DD-466C-9543-C502ADEBFECA}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECE4675-A946-4305-AAF8-D10CA956FB8A}">
   <dimension ref="A1:B71"/>
   <sheetViews>
@@ -2035,7 +2156,7 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2043,7 +2164,7 @@
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2051,7 +2172,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2059,7 +2180,7 @@
         <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2067,7 +2188,7 @@
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2075,7 +2196,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2083,7 +2204,7 @@
         <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,7 +2212,7 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2099,7 +2220,7 @@
         <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,7 +2228,7 @@
         <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2115,7 +2236,7 @@
         <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2123,7 +2244,7 @@
         <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2131,7 +2252,7 @@
         <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,7 +2260,7 @@
         <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2147,7 +2268,7 @@
         <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2155,15 +2276,15 @@
         <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2171,7 +2292,7 @@
         <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,15 +2300,15 @@
         <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2195,7 +2316,7 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2204,163 +2325,163 @@
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some flaws in special processing
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\RubberBandGun\RBG_arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F19D18-3BD2-49AA-BE53-D225861347A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150842EA-C190-4E8A-84DD-99A301531386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1680" windowWidth="32745" windowHeight="16875" activeTab="1" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="7740" yWindow="7800" windowWidth="32745" windowHeight="16875" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="146">
   <si>
     <t>trigYellow</t>
   </si>
@@ -444,12 +444,6 @@
   </si>
   <si>
     <t>new</t>
-  </si>
-  <si>
-    <t>mROW_WINDUP</t>
-  </si>
-  <si>
-    <t>… and the WINDUP</t>
   </si>
   <si>
     <t>mROW_WINDUP_SOUND</t>
@@ -962,9 +956,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E8DFC6-94F4-4A82-A874-2F16F2CF0145}">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1119,7 @@
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" t="s">
+      <c r="I4" s="11" t="s">
         <v>133</v>
       </c>
       <c r="J4" s="11"/>
@@ -1340,11 +1334,14 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>134</v>
-      </c>
       <c r="C12" t="s">
         <v>133</v>
+      </c>
+      <c r="D12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" t="s">
+        <v>134</v>
       </c>
       <c r="J12" t="s">
         <v>135</v>
@@ -1364,18 +1361,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="C14" t="s">
         <v>135</v>
       </c>
-      <c r="D14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
-      </c>
       <c r="J14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>31</v>
@@ -1385,58 +1382,52 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" t="s">
         <v>138</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" t="s">
-        <v>137</v>
+      <c r="D16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" t="s">
+        <v>140</v>
       </c>
       <c r="J16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s">
         <v>141</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" t="s">
-        <v>142</v>
-      </c>
-      <c r="J18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>145</v>
-      </c>
+      <c r="J19" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>143</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2113,7 +2104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E088660E-D1DD-466C-9543-C502ADEBFECA}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L5"/>
     </sheetView>
   </sheetViews>
@@ -2125,12 +2116,12 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
numerically sort symbols, implemnet state table for open/lock
</commit_message>
<xml_diff>
--- a/RBG_arduino/StateTable.xlsx
+++ b/RBG_arduino/StateTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdolson/GitHub-Mark-MDO47/RubberBandGun/RBG_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE57875F-5185-9D4B-886A-C6F5E6CCC2EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4570AD2-ECDD-B84D-8413-56F551D1A41D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CCADFEE4-B0E1-4363-9617-1683960BED03}"/>
   </bookViews>
   <sheets>
     <sheet name="StateTable" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -946,7 +947,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD9"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>